<commit_message>
Reformatting data variables to allow for cycling by year.
</commit_message>
<xml_diff>
--- a/_site/data/export-countries.xlsx
+++ b/_site/data/export-countries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gisselle.frias/Sites/ng-exports/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E7F34-61C0-4346-91D7-5984D1C1349B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E646D0-0B9B-5145-A039-805A957FE625}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7900" yWindow="-24820" windowWidth="30200" windowHeight="21920" xr2:uid="{29F0A3C7-455F-6046-AA29-9BAE368829E0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="88">
   <si>
     <t>countryName</t>
   </si>
@@ -281,13 +281,22 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL IN 2018  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL IN 2017  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL IN 2016  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,19 +304,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -316,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -329,11 +361,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -643,17 +703,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED965680-1F70-D243-93B5-875BC1F1D1C9}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="90.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1180,7 +1240,39 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="7">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:C36">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="2018">
+      <formula>NOT(ISERROR(SEARCH("2018",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>